<commit_message>
1st draft of D4.1 document
</commit_message>
<xml_diff>
--- a/documents/Use cases CHADA.xlsx
+++ b/documents/Use cases CHADA.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11500" windowHeight="7050" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="CHADA use cases" sheetId="1" r:id="rId1"/>
+    <sheet name=".cha attributes" sheetId="2" r:id="rId2"/>
+    <sheet name=".chag attributes" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="75">
   <si>
     <t>Use case</t>
   </si>
@@ -47,12 +49,6 @@
     <t>Decompose group of spectra</t>
   </si>
   <si>
-    <t>Statistics with gos</t>
-  </si>
-  <si>
-    <t>Extract features from gos (uni- or multivariate)</t>
-  </si>
-  <si>
     <t>Process spectrum (smooth, background, CR)</t>
   </si>
   <si>
@@ -68,62 +64,223 @@
     <t>View / explore spectrum</t>
   </si>
   <si>
-    <t>chada.plot</t>
-  </si>
-  <si>
-    <t>chada.saveplot</t>
-  </si>
-  <si>
-    <t>chada.export</t>
-  </si>
-  <si>
-    <t>chada.bands</t>
-  </si>
-  <si>
-    <t>chag.compare</t>
-  </si>
-  <si>
-    <t>chag.decompose</t>
-  </si>
-  <si>
-    <t>chag.stats</t>
-  </si>
-  <si>
-    <t>chag.features</t>
-  </si>
-  <si>
-    <t>chada.smooth, chada.back, chada.crays</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Single spectrum CHADA files contain pointer to native file, meta data, and transformers </t>
-  </si>
-  <si>
-    <t>CHADA groups interpolate single spectra on a common wavenumber axis , apply normalization and store data as numpy arrays or pandas DataFrame</t>
-  </si>
-  <si>
     <t>in Task #</t>
   </si>
   <si>
-    <t>chada.__init__</t>
-  </si>
-  <si>
-    <t>chag.__init__</t>
-  </si>
-  <si>
     <t>create CHADA group instance</t>
   </si>
   <si>
     <t>create CHADA  instance</t>
   </si>
   <si>
-    <t>chada.find</t>
+    <t>chada.__init__()</t>
+  </si>
+  <si>
+    <t>chada.plot()</t>
+  </si>
+  <si>
+    <t>chada.smooth(), chada.base(), chada.crays()</t>
+  </si>
+  <si>
+    <t>chada.saveplot()</t>
+  </si>
+  <si>
+    <t>chada.export()</t>
+  </si>
+  <si>
+    <t>chada.peaks()</t>
+  </si>
+  <si>
+    <t>chada.db_find()</t>
+  </si>
+  <si>
+    <t>chag.__init__()</t>
+  </si>
+  <si>
+    <t>chag.compare()</t>
+  </si>
+  <si>
+    <t>chag.decompose()</t>
+  </si>
+  <si>
+    <t>chag.stats()</t>
+  </si>
+  <si>
+    <t>chag.features()</t>
+  </si>
+  <si>
+    <t>Get group statistics (occurence of bands, variations)</t>
+  </si>
+  <si>
+    <t>CHADA groups interpolate CHADA spectra to a common wavenumber axis , apply normalization and store data as numpy arrays or pandas DataFrame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single spectrum CHADA files contain native data, meta data, and transformers </t>
+  </si>
+  <si>
+    <t>Extract group features (uni- or multivariate)</t>
+  </si>
+  <si>
+    <t>Fit linear regression model to known nanomarker content (target) using characteristic band intensity (univariate feature)</t>
+  </si>
+  <si>
+    <t>chag.features(), chag.LG_model.fit()</t>
+  </si>
+  <si>
+    <t>chag.normalize(), chag.features(), chag.stats()</t>
+  </si>
+  <si>
+    <t>Round Robin test comparing intensities and positions of characteristic Raman bands arising from a specific material, using measurements from different sites, instruments, and modes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'binary_data',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'filename',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'readers',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'bands',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'transformers'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'processing_state'</t>
+  </si>
+  <si>
+    <t>Positions, amplitudes etc. for most prominent Raman bands found by the peaks() method.</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Pandas DataFrame</t>
+  </si>
+  <si>
+    <t>binary stream</t>
+  </si>
+  <si>
+    <t>Native, unprocessed data and metadata</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>Name of original file</t>
+  </si>
+  <si>
+    <t>dictionary</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'metadata_static',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'metadata_dyn',</t>
+  </si>
+  <si>
+    <t>metadata extracted from native file and derived from the data upon CHADA generation</t>
+  </si>
+  <si>
+    <t>Dynamic metadata that will change upon processing</t>
+  </si>
+  <si>
+    <t>Readers corresponding to Raman native file extensions</t>
+  </si>
+  <si>
+    <t>list of CHADA transformer class instances</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fitted transformers corresponding to the processing steps that have been applied (e.g. chada.base()) </t>
+  </si>
+  <si>
+    <t>numpy array</t>
+  </si>
+  <si>
+    <t>background model (y) geenrated by the chada.base() method</t>
+  </si>
+  <si>
+    <t>State of processing, index to some element of the transformers list</t>
+  </si>
+  <si>
+    <t>Description of sample and / or experiment added by the user, or imported from an external file</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'description'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'background_model'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'filenames',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'metadatas'</t>
+  </si>
+  <si>
+    <t>list of dictionarys</t>
+  </si>
+  <si>
+    <t>metadata form the individual CHADA files included in the group</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'wavenumbers'</t>
+  </si>
+  <si>
+    <t>k axis being the intersection of all group member axes, and the minimal increment occuring in all individual axes is used for sampling.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'y_data'</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">All y data (count) vectors of the spectra in the group. Multi-dimensional data (series, maps) are serialized as lines of the y_data matrix. Data shaped in this manner can be used for a variety of machine learning models included in Python's </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ScikitLearn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> library. The original dimensionality (pixels and physical) are included in the 'metadatas' attribute.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'targets'</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>Optional known properties of the samples, such as composition or ageing state. May serve as targets for CHADA model training.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +333,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -209,36 +377,69 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -520,176 +721,469 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="A1:B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="40.6328125" customWidth="1"/>
-    <col min="2" max="2" width="27.36328125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="57" customWidth="1"/>
+    <col min="2" max="2" width="27.36328125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="11"/>
+    </row>
+    <row r="4" spans="1:3" ht="16.5" customHeight="1">
+      <c r="A4" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="14"/>
+      <c r="C4" s="13"/>
+    </row>
+    <row r="5" spans="1:3" ht="16.5" customHeight="1">
+      <c r="A5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="8"/>
+    </row>
+    <row r="7" spans="1:3" ht="29">
+      <c r="A7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="8"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="8"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="12"/>
+    </row>
+    <row r="14" spans="1:3" ht="32" customHeight="1">
+      <c r="A14" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="15"/>
+    </row>
+    <row r="15" spans="1:3" ht="19" customHeight="1">
+      <c r="A15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="4">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="8"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="8"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-    </row>
-    <row r="4" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-    </row>
-    <row r="5" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="6" t="s">
+      <c r="C18" s="8"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="11">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="3"/>
-      <c r="B12" s="6"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-    </row>
-    <row r="14" spans="1:3" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-    </row>
-    <row r="15" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="11">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>21</v>
-      </c>
+      <c r="C19" s="8"/>
+    </row>
+    <row r="20" spans="1:3" ht="29">
+      <c r="A20" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="8"/>
+    </row>
+    <row r="21" spans="1:3" ht="43.5">
+      <c r="A21" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="17.81640625" customWidth="1"/>
+    <col min="2" max="2" width="27.08984375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="44.54296875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="22.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="29">
+      <c r="A2" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="29">
+      <c r="A5" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="29">
+      <c r="A7" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="29">
+      <c r="A8" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="29">
+      <c r="A9" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="29">
+      <c r="A10" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="29">
+      <c r="A11" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:A8">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="17.81640625" customWidth="1"/>
+    <col min="2" max="2" width="16.81640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="58.6328125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="22.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="29">
+      <c r="A2" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="43.5">
+      <c r="A3" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="87">
+      <c r="A5" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="29">
+      <c r="A6" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="29">
+      <c r="A7" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="22"/>
+      <c r="B8" s="17"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="21"/>
+      <c r="B9" s="17"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="22"/>
+      <c r="B10" s="18"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="22"/>
+      <c r="B11" s="18"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>